<commit_message>
Adding BC field measurements from september-2021
</commit_message>
<xml_diff>
--- a/Campo BC com Haste Group3.xlsx
+++ b/Campo BC com Haste Group3.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARQ\Basilio\SIRIUS\Anel\Dipolos\BC-Sirius\Dipolo BC\BC-Sirius-vers2\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cnpemcamp.sharepoint.com/sites/grupoimas/Documentos Compartilhados/General/Manutenção Sirius/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61284007-090C-47EE-A584-6D7F1291E8F0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{FD91146C-8554-466F-BD9C-21A0F9B6E553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E509B710-55A5-49A0-8D88-252D7D1FBF56}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3D8BC5B1-FFE8-429A-B9D3-3A225F319967}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{3D8BC5B1-FFE8-429A-B9D3-3A225F319967}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Gráfico1" sheetId="2" r:id="rId2"/>
+    <sheet name="Gráfico temperatura" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,45 +35,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
-    <t xml:space="preserve">Campo magnético dos BCs medindo com haste sensor group 3 pelas posições atrás </t>
+    <t xml:space="preserve">Campo magnético dos BCs medido com haste sensor group 3 pelas posições atrás </t>
+  </si>
+  <si>
+    <t>Data:  04/05/2019   e   05/07/2019</t>
+  </si>
+  <si>
+    <t>Data: 27/09/2021 e 28/09/2021</t>
   </si>
   <si>
     <t xml:space="preserve">Dipolo BC </t>
   </si>
   <si>
-    <t>Entrada (gauss)</t>
+    <t>Entrada (05/2019)</t>
   </si>
   <si>
-    <t>Meio  (gauss)</t>
+    <t>Centro  (05/2019)</t>
   </si>
   <si>
-    <t>Saída  (gauss)</t>
-  </si>
-  <si>
-    <t>Data:</t>
+    <t>Saída  (05/2019)</t>
   </si>
   <si>
     <t>Temp BC</t>
   </si>
   <si>
+    <t>Entrada (09/2021)</t>
+  </si>
+  <si>
+    <t>Centro  (09/2021)</t>
+  </si>
+  <si>
+    <t>Saída  (09/2021)</t>
+  </si>
+  <si>
+    <t>dif (entrada)</t>
+  </si>
+  <si>
+    <t>dif(saída)</t>
+  </si>
+  <si>
     <t>Legenda</t>
   </si>
   <si>
-    <t>Data:  04/05/2019   e   05/07/2019</t>
+    <t>NEG ativado</t>
   </si>
   <si>
-    <t>Não medido</t>
+    <t>Em processo de ativação do NEG</t>
   </si>
   <si>
     <t>NEG não ativado</t>
   </si>
   <si>
-    <t>Em processo de ativação do NEG</t>
-  </si>
-  <si>
-    <t>NEG ativado</t>
+    <t>Não medido</t>
   </si>
 </sst>
 </file>
@@ -80,7 +98,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,12 +124,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -130,7 +142,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,56 +230,105 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -272,50 +339,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -342,7 +370,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -378,7 +406,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="pt-BR" baseline="0"/>
-              <a:t> campo do BC</a:t>
+              <a:t> campo dos BCs no Sirius</a:t>
             </a:r>
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
@@ -409,7 +437,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -438,7 +466,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Entrada (gauss)</c:v>
+                  <c:v>Entrada (05/2019)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -469,10 +497,13 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$B$4:$B$24</c:f>
+              <c:f>Planilha1!$B$4:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>9588</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>9575.5</c:v>
                 </c:pt>
@@ -526,9 +557,6 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>9441</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9588</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -536,7 +564,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-10B1-4A6A-B8FB-19307090D34F}"/>
+              <c16:uniqueId val="{00000000-CE84-4B85-947C-42E9BA2F778D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -549,7 +577,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Meio  (gauss)</c:v>
+                  <c:v>Centro  (05/2019)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -580,10 +608,13 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$C$4:$C$24</c:f>
+              <c:f>Planilha1!$C$4:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>11937</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>11923</c:v>
                 </c:pt>
@@ -637,9 +668,6 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>11741</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>11937</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -647,7 +675,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-10B1-4A6A-B8FB-19307090D34F}"/>
+              <c16:uniqueId val="{00000001-CE84-4B85-947C-42E9BA2F778D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -660,7 +688,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Saída  (gauss)</c:v>
+                  <c:v>Saída  (05/2019)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -691,10 +719,13 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$D$4:$D$24</c:f>
+              <c:f>Planilha1!$D$4:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>9587</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>9596.5</c:v>
                 </c:pt>
@@ -748,9 +779,6 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>9421</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9587</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -758,7 +786,349 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-10B1-4A6A-B8FB-19307090D34F}"/>
+              <c16:uniqueId val="{00000002-CE84-4B85-947C-42E9BA2F778D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Entrada (09/2021)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$H$4:$H$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>9505</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9513</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9470</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9524</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9495</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9533</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9493</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9507</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9502</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9518</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9492</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9532</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9522</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9510</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9504</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9509</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9506</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9539</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9512</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-CE84-4B85-947C-42E9BA2F778D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Centro  (09/2021)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$I$4:$I$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>11725</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11729</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11714</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11711</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11737</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11703</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11731</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11691</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11697</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11706</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11673</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11711</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11691</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11659</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11715</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11690</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11711</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11699</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11685</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11692</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-CE84-4B85-947C-42E9BA2F778D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Saída  (09/2021)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$J$4:$J$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>9511</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9525</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9537</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9479</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9486</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9532</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9523</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9498</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9540</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9478</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9502</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9533</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9547</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9524</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9510</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9533</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9535</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9518</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9496</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-CE84-4B85-947C-42E9BA2F778D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -802,12 +1172,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pt-BR"/>
-                  <a:t>Número</a:t>
-                </a:r>
-                <a:r>
                   <a:rPr lang="pt-BR" baseline="0"/>
-                  <a:t> BC</a:t>
+                  <a:t> BC </a:t>
                 </a:r>
                 <a:endParaRPr lang="pt-BR"/>
               </a:p>
@@ -838,10 +1204,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -875,7 +1242,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1953260272"/>
@@ -890,7 +1257,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12000"/>
-          <c:min val="9400"/>
+          <c:min val="9000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -929,7 +1296,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR"/>
-                  <a:t>Campo (Gauss)</a:t>
+                  <a:t>B (gauss)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -959,11 +1326,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -991,12 +1358,13 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1768468160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="250"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1033,7 +1401,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1070,7 +1438,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1620,10 +1988,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{19FF7E3D-5442-4992-9434-E9B535EC5556}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0021F58A-EFA7-478A-ADFD-C804C148EC3F}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -1634,13 +2002,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9646081" cy="6005593"/>
+    <xdr:ext cx="9647903" cy="6014577"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
+        <xdr:cNvPr id="3" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A464F1B3-AA18-421C-90A9-2841BD09C53A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1387A0B-6905-4771-97EA-48B0A331EDB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1664,7 +2032,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1963,1037 +2331,1591 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q48"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.28515625" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:14">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="I3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="24">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="13">
+        <v>9588</v>
+      </c>
+      <c r="C4" s="14">
+        <v>11937</v>
+      </c>
+      <c r="D4" s="14">
+        <v>9587</v>
+      </c>
+      <c r="E4" s="25"/>
+      <c r="G4" s="34">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>9505</v>
+      </c>
+      <c r="I4" s="2">
+        <v>11725</v>
+      </c>
+      <c r="J4" s="2">
+        <v>9511</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="35">
+        <f>B4-H4</f>
+        <v>83</v>
+      </c>
+      <c r="M4" s="35">
+        <f>C4-I4</f>
+        <v>212</v>
+      </c>
+      <c r="N4" s="35">
+        <f>D4-J4</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="24">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="G4" s="3">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
-        <v>2</v>
-      </c>
-      <c r="B5" s="28">
+      <c r="B5" s="13">
         <v>9575.5</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="14">
         <v>11923</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="14">
         <v>9596.5</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="G5" s="3">
+      <c r="E5" s="10"/>
+      <c r="G5" s="34">
         <f>1+G4</f>
         <v>2</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="H5" s="2">
+        <v>9513</v>
+      </c>
+      <c r="I5" s="2">
+        <v>11729</v>
+      </c>
+      <c r="J5" s="2">
+        <v>9525</v>
+      </c>
       <c r="K5" s="2"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="15" t="s">
+      <c r="L5" s="35">
+        <f>B5-H5</f>
+        <v>62.5</v>
+      </c>
+      <c r="M5" s="35">
+        <f>C5-I5</f>
+        <v>194</v>
+      </c>
+      <c r="N5" s="35">
+        <f>D5-J5</f>
+        <v>71.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="24">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13">
+        <v>9583.5</v>
+      </c>
+      <c r="C6" s="14">
+        <v>11916.5</v>
+      </c>
+      <c r="D6" s="14">
+        <v>9615</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="G6" s="34">
+        <f>1+G5</f>
+        <v>3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>9512</v>
+      </c>
+      <c r="I6" s="2">
+        <v>11714</v>
+      </c>
+      <c r="J6" s="2">
+        <v>9537</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="35">
+        <f>B6-H6</f>
+        <v>71.5</v>
+      </c>
+      <c r="M6" s="35">
+        <f>C6-I6</f>
+        <v>202.5</v>
+      </c>
+      <c r="N6" s="35">
+        <f>D6-J6</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="24">
+        <v>4</v>
+      </c>
+      <c r="B7" s="13">
+        <v>9546</v>
+      </c>
+      <c r="C7" s="14">
+        <v>11910</v>
+      </c>
+      <c r="D7" s="14">
+        <v>9558</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="G7" s="34">
+        <f>1+G6</f>
+        <v>4</v>
+      </c>
+      <c r="H7" s="2">
+        <v>9470</v>
+      </c>
+      <c r="I7" s="2">
+        <v>11711</v>
+      </c>
+      <c r="J7" s="2">
+        <v>9479</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="35">
+        <f>B7-H7</f>
+        <v>76</v>
+      </c>
+      <c r="M7" s="35">
+        <f>C7-I7</f>
+        <v>199</v>
+      </c>
+      <c r="N7" s="35">
+        <f>D7-J7</f>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="24">
+        <v>5</v>
+      </c>
+      <c r="B8" s="13">
+        <v>9607</v>
+      </c>
+      <c r="C8" s="14">
+        <v>11938</v>
+      </c>
+      <c r="D8" s="14">
+        <v>9573.5</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="G8" s="34">
+        <f>1+G7</f>
+        <v>5</v>
+      </c>
+      <c r="H8" s="2">
+        <v>9524</v>
+      </c>
+      <c r="I8" s="2">
+        <v>11737</v>
+      </c>
+      <c r="J8" s="2">
+        <v>9486</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="35">
+        <f>B8-H8</f>
+        <v>83</v>
+      </c>
+      <c r="M8" s="35">
+        <f>C8-I8</f>
+        <v>201</v>
+      </c>
+      <c r="N8" s="35">
+        <f>D8-J8</f>
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="24">
+        <v>6</v>
+      </c>
+      <c r="B9" s="13">
+        <v>9584</v>
+      </c>
+      <c r="C9" s="14">
+        <v>11908</v>
+      </c>
+      <c r="D9" s="14">
+        <v>9624</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="G9" s="34">
+        <f>1+G8</f>
+        <v>6</v>
+      </c>
+      <c r="H9" s="2">
+        <v>9495</v>
+      </c>
+      <c r="I9" s="2">
+        <v>11703</v>
+      </c>
+      <c r="J9" s="2">
+        <v>9532</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="35">
+        <f>B9-H9</f>
+        <v>89</v>
+      </c>
+      <c r="M9" s="35">
+        <f>C9-I9</f>
+        <v>205</v>
+      </c>
+      <c r="N9" s="35">
+        <f>D9-J9</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="24">
+        <v>7</v>
+      </c>
+      <c r="B10" s="13">
+        <v>9654</v>
+      </c>
+      <c r="C10" s="14">
+        <v>11961</v>
+      </c>
+      <c r="D10" s="14">
+        <v>9647</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="G10" s="34">
+        <f>1+G9</f>
+        <v>7</v>
+      </c>
+      <c r="H10" s="2">
+        <v>9533</v>
+      </c>
+      <c r="I10" s="2">
+        <v>11731</v>
+      </c>
+      <c r="J10" s="2">
+        <v>9523</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="35">
+        <f>B10-H10</f>
+        <v>121</v>
+      </c>
+      <c r="M10" s="35">
+        <f>C10-I10</f>
+        <v>230</v>
+      </c>
+      <c r="N10" s="35">
+        <f>D10-J10</f>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="24">
+        <v>8</v>
+      </c>
+      <c r="B11" s="13">
+        <v>9606.5</v>
+      </c>
+      <c r="C11" s="14">
+        <v>11916</v>
+      </c>
+      <c r="D11" s="14">
+        <v>9613</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="G11" s="34">
+        <f>1+G10</f>
+        <v>8</v>
+      </c>
+      <c r="H11" s="2">
+        <v>9493</v>
+      </c>
+      <c r="I11" s="2">
+        <v>11691</v>
+      </c>
+      <c r="J11" s="2">
+        <v>9498</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="35">
+        <f>B11-H11</f>
+        <v>113.5</v>
+      </c>
+      <c r="M11" s="35">
+        <f>C11-I11</f>
+        <v>225</v>
+      </c>
+      <c r="N11" s="35">
+        <f>D11-J11</f>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="24">
+        <v>9</v>
+      </c>
+      <c r="B12" s="13">
+        <v>9590</v>
+      </c>
+      <c r="C12" s="14">
+        <v>11895</v>
+      </c>
+      <c r="D12" s="14">
+        <v>9625</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="G12" s="34">
+        <f>1+G11</f>
+        <v>9</v>
+      </c>
+      <c r="H12" s="2">
+        <v>9507</v>
+      </c>
+      <c r="I12" s="2">
+        <v>11697</v>
+      </c>
+      <c r="J12" s="2">
+        <v>9540</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="35">
+        <f>B12-H12</f>
+        <v>83</v>
+      </c>
+      <c r="M12" s="35">
+        <f>C12-I12</f>
+        <v>198</v>
+      </c>
+      <c r="N12" s="35">
+        <f>D12-J12</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="24">
+        <v>10</v>
+      </c>
+      <c r="B13" s="13">
+        <v>9583.5</v>
+      </c>
+      <c r="C13" s="14">
+        <v>11899</v>
+      </c>
+      <c r="D13" s="14">
+        <v>9559.5</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="G13" s="34">
+        <f>1+G12</f>
+        <v>10</v>
+      </c>
+      <c r="H13" s="2">
+        <v>9502</v>
+      </c>
+      <c r="I13" s="2">
+        <v>11706</v>
+      </c>
+      <c r="J13" s="2">
+        <v>9478</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="35">
+        <f>B13-H13</f>
+        <v>81.5</v>
+      </c>
+      <c r="M13" s="35">
+        <f>C13-I13</f>
+        <v>193</v>
+      </c>
+      <c r="N13" s="35">
+        <f>D13-J13</f>
+        <v>81.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="24">
         <v>11</v>
       </c>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
-        <v>3</v>
-      </c>
-      <c r="B6" s="28">
+      <c r="B14" s="13">
         <v>9583.5</v>
       </c>
-      <c r="C6" s="29">
-        <v>11916.5</v>
-      </c>
-      <c r="D6" s="29">
-        <v>9615</v>
-      </c>
-      <c r="E6" s="23"/>
-      <c r="G6" s="3">
-        <f t="shared" ref="G6:G21" si="0">1+G5</f>
-        <v>3</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
-        <v>4</v>
-      </c>
-      <c r="B7" s="28">
-        <v>9546</v>
-      </c>
-      <c r="C7" s="29">
-        <v>11910</v>
-      </c>
-      <c r="D7" s="29">
-        <v>9558</v>
-      </c>
-      <c r="E7" s="23"/>
-      <c r="G7" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="22"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
-        <v>5</v>
-      </c>
-      <c r="B8" s="28">
-        <v>9607</v>
-      </c>
-      <c r="C8" s="29">
-        <v>11938</v>
-      </c>
-      <c r="D8" s="29">
-        <v>9573.5</v>
-      </c>
-      <c r="E8" s="23"/>
-      <c r="G8" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
-        <v>6</v>
-      </c>
-      <c r="B9" s="28">
-        <v>9584</v>
-      </c>
-      <c r="C9" s="29">
-        <v>11908</v>
-      </c>
-      <c r="D9" s="29">
-        <v>9624</v>
-      </c>
-      <c r="E9" s="23"/>
-      <c r="G9" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
-        <v>7</v>
-      </c>
-      <c r="B10" s="28">
-        <v>9654</v>
-      </c>
-      <c r="C10" s="29">
-        <v>11961</v>
-      </c>
-      <c r="D10" s="29">
-        <v>9647</v>
-      </c>
-      <c r="E10" s="23"/>
-      <c r="G10" s="3">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
-        <v>8</v>
-      </c>
-      <c r="B11" s="28">
-        <v>9606.5</v>
-      </c>
-      <c r="C11" s="29">
-        <v>11916</v>
-      </c>
-      <c r="D11" s="29">
+      <c r="C14" s="14">
+        <v>11871</v>
+      </c>
+      <c r="D14" s="14">
+        <v>9583.5</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="G14" s="34">
+        <f>1+G13</f>
+        <v>11</v>
+      </c>
+      <c r="H14" s="2">
+        <v>9518</v>
+      </c>
+      <c r="I14" s="2">
+        <v>11673</v>
+      </c>
+      <c r="J14" s="2">
+        <v>9502</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="35">
+        <f>B14-H14</f>
+        <v>65.5</v>
+      </c>
+      <c r="M14" s="35">
+        <f>C14-I14</f>
+        <v>198</v>
+      </c>
+      <c r="N14" s="35">
+        <f>D14-J14</f>
+        <v>81.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="24">
+        <v>12</v>
+      </c>
+      <c r="B15" s="13">
+        <v>9576</v>
+      </c>
+      <c r="C15" s="14">
+        <v>11889</v>
+      </c>
+      <c r="D15" s="14">
+        <v>9614</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="G15" s="34">
+        <f>1+G14</f>
+        <v>12</v>
+      </c>
+      <c r="H15" s="2">
+        <v>9492</v>
+      </c>
+      <c r="I15" s="2">
+        <v>11711</v>
+      </c>
+      <c r="J15" s="2">
+        <v>9533</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="35">
+        <f>B15-H15</f>
+        <v>84</v>
+      </c>
+      <c r="M15" s="35">
+        <f>C15-I15</f>
+        <v>178</v>
+      </c>
+      <c r="N15" s="35">
+        <f>D15-J15</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
+      <c r="B16" s="15">
+        <v>9617.5</v>
+      </c>
+      <c r="C16" s="16">
+        <v>11919</v>
+      </c>
+      <c r="D16" s="16">
+        <v>9640</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="G16" s="34">
+        <f>1+G15</f>
+        <v>13</v>
+      </c>
+      <c r="H16" s="2">
+        <v>9532</v>
+      </c>
+      <c r="I16" s="2">
+        <v>11691</v>
+      </c>
+      <c r="J16" s="2">
+        <v>9547</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="35">
+        <f>B16-H16</f>
+        <v>85.5</v>
+      </c>
+      <c r="M16" s="35">
+        <f>C16-I16</f>
+        <v>228</v>
+      </c>
+      <c r="N16" s="35">
+        <f>D16-J16</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
+      <c r="B17" s="15">
+        <v>9621</v>
+      </c>
+      <c r="C17" s="16">
+        <v>11900</v>
+      </c>
+      <c r="D17" s="16">
+        <v>9616</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="G17" s="34">
+        <f>1+G16</f>
+        <v>14</v>
+      </c>
+      <c r="H17" s="2">
+        <v>9522</v>
+      </c>
+      <c r="I17" s="2">
+        <v>11659</v>
+      </c>
+      <c r="J17" s="2">
+        <v>9524</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="35">
+        <f>B17-H17</f>
+        <v>99</v>
+      </c>
+      <c r="M17" s="35">
+        <f>C17-I17</f>
+        <v>241</v>
+      </c>
+      <c r="N17" s="35">
+        <f>D17-J17</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="19">
+        <v>15</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22"/>
+      <c r="G18" s="34">
+        <f>1+G17</f>
+        <v>15</v>
+      </c>
+      <c r="H18" s="2">
+        <v>9510</v>
+      </c>
+      <c r="I18" s="2">
+        <v>11715</v>
+      </c>
+      <c r="J18" s="2">
+        <v>9500</v>
+      </c>
+      <c r="K18" s="2"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="9">
+        <v>16</v>
+      </c>
+      <c r="B19" s="15">
+        <v>9572.5</v>
+      </c>
+      <c r="C19" s="16">
+        <v>11889</v>
+      </c>
+      <c r="D19" s="16">
+        <v>9598.5</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="G19" s="34">
+        <f>1+G18</f>
+        <v>16</v>
+      </c>
+      <c r="H19" s="2">
+        <v>9504</v>
+      </c>
+      <c r="I19" s="2">
+        <v>11690</v>
+      </c>
+      <c r="J19" s="2">
+        <v>9510</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="L19" s="35">
+        <f>B19-H19</f>
+        <v>68.5</v>
+      </c>
+      <c r="M19" s="35">
+        <f>C19-I19</f>
+        <v>199</v>
+      </c>
+      <c r="N19" s="35">
+        <f>D19-J19</f>
+        <v>88.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="9">
+        <v>17</v>
+      </c>
+      <c r="B20" s="15">
+        <v>9585</v>
+      </c>
+      <c r="C20" s="16">
+        <v>11911.5</v>
+      </c>
+      <c r="D20" s="16">
         <v>9613</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="G11" s="3">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="O11" s="11"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
-        <v>9</v>
-      </c>
-      <c r="B12" s="28">
-        <v>9590</v>
-      </c>
-      <c r="C12" s="29">
-        <v>11895</v>
-      </c>
-      <c r="D12" s="29">
-        <v>9625</v>
-      </c>
-      <c r="E12" s="23"/>
-      <c r="G12" s="3">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
-        <v>10</v>
-      </c>
-      <c r="B13" s="28">
-        <v>9583.5</v>
-      </c>
-      <c r="C13" s="29">
-        <v>11899</v>
-      </c>
-      <c r="D13" s="29">
-        <v>9559.5</v>
-      </c>
-      <c r="E13" s="23"/>
-      <c r="G13" s="3">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
-        <v>11</v>
-      </c>
-      <c r="B14" s="28">
-        <v>9583.5</v>
-      </c>
-      <c r="C14" s="29">
-        <v>11871</v>
-      </c>
-      <c r="D14" s="29">
-        <v>9583.5</v>
-      </c>
-      <c r="E14" s="23"/>
-      <c r="G14" s="3">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
-        <v>12</v>
-      </c>
-      <c r="B15" s="28">
-        <v>9576</v>
-      </c>
-      <c r="C15" s="29">
-        <v>11889</v>
-      </c>
-      <c r="D15" s="29">
-        <v>9614</v>
-      </c>
-      <c r="E15" s="23"/>
-      <c r="G15" s="3">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="18">
-        <v>13</v>
-      </c>
-      <c r="B16" s="30">
-        <v>9617.5</v>
-      </c>
-      <c r="C16" s="31">
-        <v>11919</v>
-      </c>
-      <c r="D16" s="31">
-        <v>9640</v>
-      </c>
-      <c r="E16" s="24"/>
-      <c r="G16" s="3">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="18">
-        <v>14</v>
-      </c>
-      <c r="B17" s="30">
-        <v>9621</v>
-      </c>
-      <c r="C17" s="31">
-        <v>11900</v>
-      </c>
-      <c r="D17" s="31">
+      <c r="E20" s="11"/>
+      <c r="G20" s="34">
+        <f>1+G19</f>
+        <v>17</v>
+      </c>
+      <c r="H20" s="2">
+        <v>9509</v>
+      </c>
+      <c r="I20" s="2">
+        <v>11711</v>
+      </c>
+      <c r="J20" s="2">
+        <v>9533</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" s="35">
+        <f>B20-H20</f>
+        <v>76</v>
+      </c>
+      <c r="M20" s="35">
+        <f>C20-I20</f>
+        <v>200.5</v>
+      </c>
+      <c r="N20" s="35">
+        <f>D20-J20</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="9">
+        <v>18</v>
+      </c>
+      <c r="B21" s="15">
+        <v>9589.5</v>
+      </c>
+      <c r="C21" s="16">
+        <v>11905</v>
+      </c>
+      <c r="D21" s="16">
         <v>9616</v>
       </c>
-      <c r="E17" s="24"/>
-      <c r="G17" s="3">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
-        <v>15</v>
-      </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="25"/>
-      <c r="G18" s="3">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="18">
-        <v>16</v>
-      </c>
-      <c r="B19" s="30">
-        <v>9572.5</v>
-      </c>
-      <c r="C19" s="31">
-        <v>11889</v>
-      </c>
-      <c r="D19" s="31">
+      <c r="E21" s="11"/>
+      <c r="G21" s="34">
+        <f>1+G20</f>
+        <v>18</v>
+      </c>
+      <c r="H21" s="2">
+        <v>9506</v>
+      </c>
+      <c r="I21" s="2">
+        <v>11699</v>
+      </c>
+      <c r="J21" s="2">
+        <v>9535</v>
+      </c>
+      <c r="K21" s="2"/>
+      <c r="L21" s="35">
+        <f>B21-H21</f>
+        <v>83.5</v>
+      </c>
+      <c r="M21" s="35">
+        <f>C21-I21</f>
+        <v>206</v>
+      </c>
+      <c r="N21" s="35">
+        <f>D21-J21</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="9">
+        <v>19</v>
+      </c>
+      <c r="B22" s="15">
+        <v>9616</v>
+      </c>
+      <c r="C22" s="16">
+        <v>11898</v>
+      </c>
+      <c r="D22" s="16">
         <v>9598.5</v>
       </c>
-      <c r="E19" s="24"/>
-      <c r="G19" s="3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="18">
-        <v>17</v>
-      </c>
-      <c r="B20" s="30">
-        <v>9585</v>
-      </c>
-      <c r="C20" s="31">
-        <v>11911.5</v>
-      </c>
-      <c r="D20" s="31">
-        <v>9613</v>
-      </c>
-      <c r="E20" s="24"/>
-      <c r="G20" s="3">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="18">
-        <v>18</v>
-      </c>
-      <c r="B21" s="30">
-        <v>9589.5</v>
-      </c>
-      <c r="C21" s="31">
-        <v>11905</v>
-      </c>
-      <c r="D21" s="31">
-        <v>9616</v>
-      </c>
-      <c r="E21" s="24"/>
-      <c r="G21" s="3">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="18">
-        <v>19</v>
-      </c>
-      <c r="B22" s="30">
-        <v>9616</v>
-      </c>
-      <c r="C22" s="31">
-        <v>11898</v>
-      </c>
-      <c r="D22" s="31">
-        <v>9598.5</v>
-      </c>
-      <c r="E22" s="24"/>
-      <c r="G22" s="3">
+      <c r="E22" s="11"/>
+      <c r="G22" s="34">
         <f>1+G21</f>
         <v>19</v>
       </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+      <c r="H22" s="2">
+        <v>9539</v>
+      </c>
+      <c r="I22" s="2">
+        <v>11685</v>
+      </c>
+      <c r="J22" s="2">
+        <v>9518</v>
+      </c>
       <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
+      <c r="L22" s="35">
+        <f>B22-H22</f>
+        <v>77</v>
+      </c>
+      <c r="M22" s="35">
+        <f>C22-I22</f>
+        <v>213</v>
+      </c>
+      <c r="N22" s="35">
+        <f>D22-J22</f>
+        <v>80.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="5">
         <v>20</v>
       </c>
-      <c r="B23" s="34">
+      <c r="B23" s="17">
         <v>9441</v>
       </c>
-      <c r="C23" s="35">
+      <c r="C23" s="18">
         <v>11741</v>
       </c>
-      <c r="D23" s="35">
+      <c r="D23" s="18">
         <v>9421</v>
       </c>
-      <c r="E23" s="26"/>
-      <c r="G23" s="3">
-        <f t="shared" ref="G23:G24" si="1">1+G22</f>
+      <c r="E23" s="12"/>
+      <c r="G23" s="34">
+        <f>1+G22</f>
         <v>20</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
+      <c r="H23" s="2">
+        <v>9512</v>
+      </c>
+      <c r="I23" s="2">
+        <v>11692</v>
+      </c>
+      <c r="J23" s="2">
+        <v>9496</v>
+      </c>
       <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="19">
-        <v>21</v>
-      </c>
-      <c r="B24" s="36">
-        <v>9588</v>
-      </c>
-      <c r="C24" s="37">
-        <v>11937</v>
-      </c>
-      <c r="D24" s="37">
-        <v>9587</v>
-      </c>
-      <c r="E24" s="27"/>
-      <c r="G24" s="3">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>1</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="G28" s="3">
-        <v>1</v>
-      </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <f>1+A28</f>
-        <v>2</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="G29" s="3">
-        <f>1+G28</f>
-        <v>2</v>
-      </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <f t="shared" ref="A30:A45" si="2">1+A29</f>
-        <v>3</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="G30" s="3">
-        <f t="shared" ref="G30:G45" si="3">1+G29</f>
-        <v>3</v>
-      </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="G31" s="3">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="G32" s="3">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="G33" s="3">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="G34" s="3">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
+      <c r="L23" s="35">
+        <f>B23-H23</f>
+        <v>-71</v>
+      </c>
+      <c r="M23" s="35">
+        <f>C23-I23</f>
+        <v>49</v>
+      </c>
+      <c r="N23" s="35">
+        <f>D23-J23</f>
+        <v>-75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="28"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="31"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="6"/>
+      <c r="B26" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="7"/>
+      <c r="B27" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="8"/>
+      <c r="B28" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="23"/>
+      <c r="B29" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="41"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="31"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="27"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="38"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="32"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="4"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="26"/>
+      <c r="M34" s="26"/>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="34"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
-      <c r="G35" s="3">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
+      <c r="G35" s="34"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
+      <c r="L35" s="27"/>
+      <c r="M35" s="27"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="34"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
-      <c r="G36" s="3">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
+      <c r="G36" s="34"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="34"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
-      <c r="G37" s="3">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
+      <c r="G37" s="34"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
+      <c r="L37" s="27"/>
+      <c r="M37" s="27"/>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="34"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
-      <c r="G38" s="3">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
+      <c r="G38" s="34"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="34"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
-      <c r="G39" s="3">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
+      <c r="G39" s="34"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
+      <c r="L39" s="27"/>
+      <c r="M39" s="27"/>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="34"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
-      <c r="G40" s="3">
-        <f t="shared" si="3"/>
-        <v>13</v>
-      </c>
+      <c r="G40" s="34"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="34"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
-      <c r="G41" s="3">
-        <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
+      <c r="G41" s="34"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
+      <c r="L41" s="27"/>
+      <c r="M41" s="27"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="34"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
-      <c r="G42" s="3">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
+      <c r="G42" s="34"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
+      <c r="L42" s="27"/>
+      <c r="M42" s="27"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="34"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
-      <c r="G43" s="3">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
+      <c r="G43" s="34"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
+      <c r="L43" s="27"/>
+      <c r="M43" s="27"/>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="34"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
-      <c r="G44" s="3">
-        <f t="shared" si="3"/>
-        <v>17</v>
-      </c>
+      <c r="G44" s="34"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
+      <c r="L44" s="27"/>
+      <c r="M44" s="27"/>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="34"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
-      <c r="G45" s="3">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
+      <c r="G45" s="34"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
-        <f>1+A45</f>
-        <v>19</v>
-      </c>
+      <c r="L45" s="27"/>
+      <c r="M45" s="27"/>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="34"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
-      <c r="G46" s="3">
-        <f>1+G45</f>
-        <v>19</v>
-      </c>
+      <c r="G46" s="34"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
-        <f t="shared" ref="A47:A48" si="4">1+A46</f>
-        <v>20</v>
-      </c>
+      <c r="L46" s="27"/>
+      <c r="M46" s="27"/>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="34"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
-      <c r="G47" s="3">
-        <f t="shared" ref="G47:G48" si="5">1+G46</f>
-        <v>20</v>
-      </c>
+      <c r="G47" s="34"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
-        <f t="shared" si="4"/>
-        <v>21</v>
-      </c>
+      <c r="L47" s="27"/>
+      <c r="M47" s="27"/>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="34"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
-      <c r="G48" s="3">
-        <f t="shared" si="5"/>
-        <v>21</v>
-      </c>
+      <c r="G48" s="34"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
+      <c r="L48" s="27"/>
+      <c r="M48" s="27"/>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="34"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="G49" s="34"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="27"/>
+      <c r="M49" s="27"/>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="34"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="G50" s="34"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="27"/>
+      <c r="M50" s="27"/>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="34"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="G51" s="34"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="27"/>
+      <c r="M51" s="27"/>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="34"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="G52" s="34"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="27"/>
+      <c r="M52" s="27"/>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="34"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="27"/>
+      <c r="M53" s="27"/>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="34"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="G54" s="34"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="27"/>
+      <c r="M54" s="27"/>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="34"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="G55" s="34"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="27"/>
+      <c r="M55" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="G26:K26"/>
-    <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="M3:Q3"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="N4:Q4"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="G2:K2"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="G33:K33"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B26:E26"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="82" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="59" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007A7E416D919B234B9674A954BD75FE26" ma:contentTypeVersion="9" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="732e1eee9d76b5142dbae3a81082dbc8">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dfe0e87d-c18b-4fe8-a38f-f5371de371f3" xmlns:ns3="2d1c0536-4bd1-4da3-8d9b-e331e956cbc8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="10d811aa86ef12152b3743135c99fc5c" ns2:_="" ns3:_="">
+    <xsd:import namespace="dfe0e87d-c18b-4fe8-a38f-f5371de371f3"/>
+    <xsd:import namespace="2d1c0536-4bd1-4da3-8d9b-e331e956cbc8"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="dfe0e87d-c18b-4fe8-a38f-f5371de371f3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="11" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="12" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2d1c0536-4bd1-4da3-8d9b-e331e956cbc8" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Compartilhado com" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Detalhes de Compartilhado Com" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de Conteúdo"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5527C09E-379E-4757-BF52-93E6FDCCA789}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDD9E22E-5DCA-4D76-99F6-949319FDA9B6}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10A0A6AE-BDF3-4C7E-95D8-42D3AD76675C}"/>
 </file>
</xml_diff>